<commit_message>
incomplete fix of demo
</commit_message>
<xml_diff>
--- a/data/demo/factories/cementFactory.xlsx
+++ b/data/demo/factories/cementFactory.xlsx
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="cementFactoryChains" localSheetId="0">'Chain List'!$A$1:$D$3</definedName>
-    <definedName name="cementFactoryConnections" localSheetId="1">Connections!$B$1:$F$2</definedName>
+    <definedName name="cementFactoryConnections" localSheetId="1">Connections!$A$1:$G$2</definedName>
     <definedName name="cementFlow" localSheetId="2">'Cement Chain'!$A$1:$C$4</definedName>
     <definedName name="powerFlow" localSheetId="3">'Power Chain'!$A$1:$C$2</definedName>
   </definedNames>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
   <si>
     <t>ChainName</t>
   </si>
@@ -110,15 +110,6 @@
     <t>ChainSheet</t>
   </si>
   <si>
-    <t>Product</t>
-  </si>
-  <si>
-    <t>Product_IO_of_Origin</t>
-  </si>
-  <si>
-    <t>Product_IO_of_Destination</t>
-  </si>
-  <si>
     <t>all</t>
   </si>
   <si>
@@ -152,27 +143,6 @@
     <t>same</t>
   </si>
   <si>
-    <t>Recycle_Replacing</t>
-  </si>
-  <si>
-    <t>Purge_Fraction</t>
-  </si>
-  <si>
-    <t>Origin_Unit</t>
-  </si>
-  <si>
-    <t>Destination_Unit</t>
-  </si>
-  <si>
-    <t>Origin_Chain</t>
-  </si>
-  <si>
-    <t>Destination_Chain</t>
-  </si>
-  <si>
-    <t>Max_Replace_Fraction</t>
-  </si>
-  <si>
     <t>waste heat</t>
   </si>
   <si>
@@ -189,6 +159,39 @@
   </si>
   <si>
     <t>demo_powerstation</t>
+  </si>
+  <si>
+    <t>o chain</t>
+  </si>
+  <si>
+    <t>o unit</t>
+  </si>
+  <si>
+    <t>o flowtype</t>
+  </si>
+  <si>
+    <t>d chain</t>
+  </si>
+  <si>
+    <t>d flowtype</t>
+  </si>
+  <si>
+    <t>r replacing</t>
+  </si>
+  <si>
+    <t>d unit</t>
+  </si>
+  <si>
+    <t>r purge %</t>
+  </si>
+  <si>
+    <t>r max replace %</t>
+  </si>
+  <si>
+    <t>o product</t>
+  </si>
+  <si>
+    <t>d product</t>
   </si>
 </sst>
 </file>
@@ -599,10 +602,10 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -616,10 +619,10 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -629,108 +632,118 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5" customWidth="1"/>
-    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>28</v>
       </c>
       <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -751,43 +764,43 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -815,21 +828,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>

</xml_diff>